<commit_message>
BIC is now defined as matrix, with index names and column names
</commit_message>
<xml_diff>
--- a/BIC.xlsx
+++ b/BIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\_PVT karakterizacija\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5338AA5-97FA-4EDD-98CA-C613893076F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2119B1-B2BD-4219-8B14-6B9680AFBFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="16440" xr2:uid="{F627E816-A48A-43B3-A51A-E3D621316A99}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
   <si>
     <t>N2</t>
   </si>
@@ -1105,602 +1105,65 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>0.02</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="D1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="E1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="F1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="G1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="I1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="J1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="K1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="L1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="M1" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412C7C25-1081-4E59-B023-AA575A7599AC}">
-  <dimension ref="A1:O32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1717,6 +1180,490 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412C7C25-1081-4E59-B023-AA575A7599AC}">
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>

</xml_diff>